<commit_message>
added the logic for data scraping and storing
</commit_message>
<xml_diff>
--- a/Excel-uri Comparare Preturi/Model Mapare Coduri2_StorePriceCompare.xlsx
+++ b/Excel-uri Comparare Preturi/Model Mapare Coduri2_StorePriceCompare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bahna\Desktop\Excel-uri Comparare Preturi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dragos\Documents\UiPath\RPA\Excel-uri Comparare Preturi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA55AFC-1CDE-4334-880B-CAF1AE001B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD43637-017F-4A74-81DF-4A2798702013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{613F1637-A29C-4AA0-AE5C-7A8FE6123CD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{613F1637-A29C-4AA0-AE5C-7A8FE6123CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Coduri" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Atomico</t>
   </si>
@@ -43,41 +43,62 @@
     <t>example@domain.com</t>
   </si>
   <si>
-    <t>YT-3286</t>
-  </si>
-  <si>
-    <t>THT7143206</t>
-  </si>
-  <si>
-    <t>WFS4100</t>
-  </si>
-  <si>
-    <t>HECHT546BSW</t>
-  </si>
-  <si>
-    <t>YT-84900</t>
-  </si>
-  <si>
     <t>Locatie Finala:</t>
   </si>
   <si>
     <t>C:\Users\Desktop\Cristian\</t>
   </si>
   <si>
-    <t>TAC312003C</t>
-  </si>
-  <si>
-    <t>WFS058.PACHET</t>
-  </si>
-  <si>
-    <t>DAX6000.PACHET-4</t>
+    <t>TAC312003C &lt;-&gt; 45.10</t>
+  </si>
+  <si>
+    <t>YT-3286 &lt;-&gt; 28.00</t>
+  </si>
+  <si>
+    <t>100369442 &lt;-&gt; 29.00</t>
+  </si>
+  <si>
+    <t>THT7143206 &lt;-&gt; 70.46</t>
+  </si>
+  <si>
+    <t>30510 &lt;-&gt; 43.00</t>
+  </si>
+  <si>
+    <t>100626185 &lt;-&gt; 52.00</t>
+  </si>
+  <si>
+    <t>WFS058.PACHET &lt;-&gt; 299.00</t>
+  </si>
+  <si>
+    <t>79076 &lt;-&gt; 288.00</t>
+  </si>
+  <si>
+    <t>100667048 &lt;-&gt; 449.00</t>
+  </si>
+  <si>
+    <t>WFS4100 &lt;-&gt; 1009.36</t>
+  </si>
+  <si>
+    <t>HECHT546BSW &lt;-&gt; 1637.20</t>
+  </si>
+  <si>
+    <t>101072293 &lt;-&gt; 1279.00</t>
+  </si>
+  <si>
+    <t>DAX6000.PACHET-4 &lt;-&gt; 554.00</t>
+  </si>
+  <si>
+    <t>YT-84900 &lt;-&gt; 616.00</t>
+  </si>
+  <si>
+    <t>100646740 &lt;-&gt; 449.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +124,39 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDC143C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF228B22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8C00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,6 +181,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,15 +505,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,59 +524,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100369442</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>30510</v>
-      </c>
-      <c r="C3" s="1">
-        <v>100626185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
-        <v>79076</v>
-      </c>
-      <c r="C4" s="1">
-        <v>100667048</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>101072293</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>100646740</v>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -542,13 +592,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -556,12 +606,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>